<commit_message>
algoritmo genetico funcionando TO DO: {} agregar al calculo de la distancia el regreso a la primera ciudad al igual que a la generacion de individuos ??? el algoritmo se sale del maximo y cae en un mimnimo local
</commit_message>
<xml_diff>
--- a/Ciudades.xlsx
+++ b/Ciudades.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27930"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28004"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="85" documentId="8_{A2C0C8CA-44CB-4392-85FF-5A07803A2BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{635F7F34-D3C6-4672-A6D6-03F983FA3757}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="8_{A2C0C8CA-44CB-4392-85FF-5A07803A2BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2BDCE6F-0C61-4077-B631-AC49F2CF40E6}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -280,6 +280,1206 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>"y"</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!C1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$2:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$C$2:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{D3E1D990-6E8F-4712-B399-DACCF54150D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="660336135"/>
+        <c:axId val="1698289160"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="660336135"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>x</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1698289160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="30"/>
+        <c:minorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1698289160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>y</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="660336135"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="30"/>
+        <c:minorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1" descr="Tipo de gráfico: Dispersión. &quot;y&quot;&#10;&#10;Descripción generada automáticamente">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A85833F-A98A-9653-F443-68EBF1D9C164}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -602,7 +1802,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -669,57 +1869,89 @@
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="3">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="3">
+        <v>53</v>
+      </c>
+      <c r="C7" s="3">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="3">
+        <v>39</v>
+      </c>
+      <c r="C8" s="3">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="3">
+        <v>45</v>
+      </c>
+      <c r="C9" s="3">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="B10" s="4">
+        <v>61</v>
+      </c>
+      <c r="C10" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="4">
+        <v>69</v>
+      </c>
+      <c r="C11" s="4">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="4">
+        <v>78</v>
+      </c>
+      <c r="C12" s="4">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="B13" s="4">
+        <v>85</v>
+      </c>
+      <c r="C13" s="4">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="5" t="s">
@@ -899,6 +2131,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -912,6 +2145,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d70ee3a7-4447-42b6-87f5-b089beab3fa2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="050d698c-19bf-401f-b68f-1964349f79d6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFF27E4D1B175E4EB1652F7A40982A6F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7f361dbe96de01fb6b84c35138e9cbd8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="050d698c-19bf-401f-b68f-1964349f79d6" xmlns:ns3="d70ee3a7-4447-42b6-87f5-b089beab3fa2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="12e70d55eb5aeefa8b7f3bc64fad5a2a" ns2:_="" ns3:_="">
     <xsd:import namespace="050d698c-19bf-401f-b68f-1964349f79d6"/>
@@ -1106,25 +2350,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d70ee3a7-4447-42b6-87f5-b089beab3fa2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="050d698c-19bf-401f-b68f-1964349f79d6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FEA17DC-BE29-40CE-BB88-DF80048A5F3C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8302D570-D0C7-4FA2-BAEC-5DAA5BE0787D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F511A11-F9F8-449A-B594-80A14AFEA8B9}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F511A11-F9F8-449A-B594-80A14AFEA8B9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8302D570-D0C7-4FA2-BAEC-5DAA5BE0787D}"/>
 </file>
</xml_diff>